<commit_message>
📁 Add route to download Excel file
</commit_message>
<xml_diff>
--- a/contact_data_.xlsx
+++ b/contact_data_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bssha\Downloads\protfolio_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B2B017-AC26-4BA8-9AE4-3539D8123884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A26B0D-E183-4539-BF25-1E09FEB9D6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,17 +417,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="38.09765625" customWidth="1"/>
     <col min="3" max="3" width="35.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>